<commit_message>
Added sort python code
</commit_message>
<xml_diff>
--- a/assigns/TeamEvals.xlsx
+++ b/assigns/TeamEvals.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23117"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20700" windowHeight="15480" tabRatio="500"/>
+    <workbookView xWindow="1960" yWindow="560" windowWidth="23780" windowHeight="19340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="75">
   <si>
     <t>1- completely disagree</t>
   </si>
@@ -230,6 +230,21 @@
   </si>
   <si>
     <t>Overall</t>
+  </si>
+  <si>
+    <t>Teammate #1</t>
+  </si>
+  <si>
+    <t>Teammate #2</t>
+  </si>
+  <si>
+    <t>Teammate #3</t>
+  </si>
+  <si>
+    <t>Own Contributions</t>
+  </si>
+  <si>
+    <t>Describe the contributions of your teammates here:</t>
   </si>
 </sst>
 </file>
@@ -320,7 +335,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -365,8 +380,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -398,8 +428,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -421,8 +461,13 @@
     <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="41">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -438,6 +483,11 @@
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -453,6 +503,11 @@
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="11">
@@ -983,16 +1038,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14" style="6" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.33203125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" style="6" customWidth="1"/>
     <col min="3" max="3" width="89.5" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="7" width="12.1640625" style="3" customWidth="1"/>
     <col min="8" max="8" width="10.83203125" style="3"/>
@@ -1006,10 +1061,9 @@
       <c r="B1" s="5"/>
     </row>
     <row r="3" spans="1:7" ht="20">
-      <c r="A3" s="7" t="s">
+      <c r="B3" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="7"/>
       <c r="C3" s="3" t="s">
         <v>61</v>
       </c>
@@ -1333,6 +1387,35 @@
       <c r="C36" s="2" t="s">
         <v>32</v>
       </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="B40" s="13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="109" customHeight="1">
+      <c r="B41" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C41" s="15"/>
+    </row>
+    <row r="42" spans="1:3" ht="108" customHeight="1">
+      <c r="B42" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="C42" s="15"/>
+    </row>
+    <row r="43" spans="1:3" ht="109" customHeight="1">
+      <c r="B43" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C43" s="15"/>
+    </row>
+    <row r="44" spans="1:3" ht="107" customHeight="1">
+      <c r="B44" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C44" s="15"/>
     </row>
   </sheetData>
   <sortState ref="C13:I32">

</xml_diff>